<commit_message>
Separated Notebooks by sport
</commit_message>
<xml_diff>
--- a/NBA_Basketball_Monday_3.21_LATE_GAME_CHANGES.xlsx
+++ b/NBA_Basketball_Monday_3.21_LATE_GAME_CHANGES.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Best Sports Book(HT)</t>
   </si>
@@ -37,22 +37,28 @@
     <t>id</t>
   </si>
   <si>
-    <t>FanDuel</t>
+    <t>Unibet</t>
+  </si>
+  <si>
+    <t>SugarHouse</t>
+  </si>
+  <si>
+    <t>GTbets</t>
+  </si>
+  <si>
+    <t>TwinSpires</t>
+  </si>
+  <si>
+    <t>William Hill (US)</t>
+  </si>
+  <si>
+    <t>BetMGM</t>
   </si>
   <si>
     <t>WynnBET</t>
   </si>
   <si>
-    <t>BetRivers</t>
-  </si>
-  <si>
-    <t>William Hill (US)</t>
-  </si>
-  <si>
-    <t>TwinSpires</t>
-  </si>
-  <si>
-    <t>LowVig.ag</t>
+    <t>BetOnline.ag</t>
   </si>
   <si>
     <t>Charlotte Hornets</t>
@@ -61,52 +67,52 @@
     <t>Cleveland Cavaliers</t>
   </si>
   <si>
-    <t>Detroit Pistons</t>
-  </si>
-  <si>
-    <t>Brooklyn Nets</t>
+    <t>Atlanta Hawks</t>
+  </si>
+  <si>
+    <t>Boston Celtics</t>
+  </si>
+  <si>
+    <t>Chicago Bulls</t>
   </si>
   <si>
     <t>Miami Heat</t>
   </si>
   <si>
-    <t>Boston Celtics</t>
-  </si>
-  <si>
-    <t>Chicago Bulls</t>
-  </si>
-  <si>
     <t>Houston Rockets</t>
   </si>
   <si>
-    <t>Dallas Mavericks</t>
-  </si>
-  <si>
-    <t>New Orleans Pelicans</t>
-  </si>
-  <si>
-    <t>Los Angeles Lakers</t>
+    <t>Golden State Warriors</t>
+  </si>
+  <si>
+    <t>Oklahoma City Thunder</t>
+  </si>
+  <si>
+    <t>Denver Nuggets</t>
+  </si>
+  <si>
+    <t>Orlando Magic</t>
+  </si>
+  <si>
+    <t>Indiana Pacers</t>
+  </si>
+  <si>
+    <t>Toronto Raptors</t>
+  </si>
+  <si>
+    <t>New York Knicks</t>
+  </si>
+  <si>
+    <t>Sacramento Kings</t>
+  </si>
+  <si>
+    <t>San Antonio Spurs</t>
+  </si>
+  <si>
+    <t>Memphis Grizzlies</t>
   </si>
   <si>
     <t>Portland Trail Blazers</t>
-  </si>
-  <si>
-    <t>Utah Jazz</t>
-  </si>
-  <si>
-    <t>Philadelphia 76ers</t>
-  </si>
-  <si>
-    <t>Oklahoma City Thunder</t>
-  </si>
-  <si>
-    <t>Toronto Raptors</t>
-  </si>
-  <si>
-    <t>Washington Wizards</t>
-  </si>
-  <si>
-    <t>Minnesota Timberwolves</t>
   </si>
 </sst>
 </file>
@@ -501,19 +507,19 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>-4</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -524,19 +530,19 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>-4.5</v>
+        <v>-9.5</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3">
-        <v>4.5</v>
+        <v>9.5</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -544,22 +550,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>-7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>-10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -567,22 +573,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F5">
-        <v>-2</v>
+        <v>-3.5</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -590,22 +596,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6">
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -613,22 +619,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7">
-        <v>-14.5</v>
+        <v>-13.5</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F7">
-        <v>14.5</v>
+        <v>13.5</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -636,22 +642,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D8">
-        <v>-4</v>
+        <v>6.5</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>-6.5</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -659,22 +665,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>10.5</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F9">
-        <v>-5</v>
+        <v>-10.5</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -682,22 +688,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>-2</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>